<commit_message>
ajout affichage heure debut
</commit_message>
<xml_diff>
--- a/tableau2.xlsx
+++ b/tableau2.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1352,6 +1352,348 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2,2077215917241975</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2,1794148056623137</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>23,685714285714287</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2,223611367075916</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2,2048816641098052</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>23,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2,2146582486515953</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2,1954575391601954</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>23,714285714285715</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2,235946882498052</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2,223201451371017</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>17,685714285714287</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2,2511713964947746</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2,2385759327792862</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>17,214285714285715</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>(0, 0,1)</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0,40360077396405736</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0,37413761358399433</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>89,62857142857143</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>